<commit_message>
Refactor codes (create 2 Services)
</commit_message>
<xml_diff>
--- a/Service_API_front/FrontEnd_API.xlsx
+++ b/Service_API_front/FrontEnd_API.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramin\PycharmProjects\Mohaddes_InstagramAPI\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ramin\PycharmProjects\Mohaddes_InstagramAPI\Service_API_front\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE213AA7-73D7-421E-A55E-3F63D2484A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC741F30-2A1C-470B-9842-A3904689A2F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{4109CEAF-297B-4EAE-8365-951A3060F5F6}"/>
   </bookViews>
@@ -39,9 +39,6 @@
     <t>Api</t>
   </si>
   <si>
-    <t xml:space="preserve">         trueExploreMode: string,</t>
-  </si>
-  <si>
     <t xml:space="preserve">         contentType: string[],</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">         trueExploreMode: bool,</t>
   </si>
 </sst>
 </file>
@@ -509,7 +509,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -525,163 +525,163 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>19</v>
+      </c>
+      <c r="D1" t="s">
         <v>20</v>
-      </c>
-      <c r="D1" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="19.8" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>1</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>